<commit_message>
operational without all safety measures
</commit_message>
<xml_diff>
--- a/backup/testWorksheetBackup.xlsx
+++ b/backup/testWorksheetBackup.xlsx
@@ -19710,7 +19710,7 @@
         </is>
       </c>
       <c r="B9" s="131" t="n">
-        <v>30308.14</v>
+        <v>30335.67</v>
       </c>
       <c r="C9" s="74" t="n">
         <v>2</v>
@@ -19940,7 +19940,7 @@
         </is>
       </c>
       <c r="B10" s="131" t="n">
-        <v>3730.31</v>
+        <v>3727.04</v>
       </c>
       <c r="C10" s="74">
         <f>C9+1</f>
@@ -20171,7 +20171,7 @@
         </is>
       </c>
       <c r="B11" s="131" t="n">
-        <v>12855.5</v>
+        <v>12866.32</v>
       </c>
       <c r="C11" s="74">
         <f>C10+1</f>
@@ -20402,7 +20402,7 @@
         </is>
       </c>
       <c r="B12" s="131" t="n">
-        <v>1955.08</v>
+        <v>1955.26</v>
       </c>
       <c r="C12" s="74">
         <f>C11+1</f>
@@ -20633,7 +20633,7 @@
         </is>
       </c>
       <c r="B13" s="131" t="n">
-        <v>2710.2</v>
+        <v>2714.21</v>
       </c>
       <c r="C13" s="74">
         <f>C12+1</f>
@@ -21827,7 +21827,9 @@
           <t>BOVESPA (Brazil)</t>
         </is>
       </c>
-      <c r="B19" s="131" t="n"/>
+      <c r="B19" s="131" t="n">
+        <v>119409.15</v>
+      </c>
       <c r="C19" s="74">
         <f>C18+1</f>
         <v/>
@@ -22049,7 +22051,9 @@
           <t>MSCI Emg Mkts (USD)</t>
         </is>
       </c>
-      <c r="B20" s="131" t="n"/>
+      <c r="B20" s="131" t="n">
+        <v>1252.33</v>
+      </c>
       <c r="C20" s="74">
         <f>C19+1</f>
         <v/>
@@ -22271,7 +22275,9 @@
           <t>WSJ Dollar Index</t>
         </is>
       </c>
-      <c r="B21" s="131" t="n"/>
+      <c r="B21" s="131" t="n">
+        <v>85.20999999999999</v>
+      </c>
       <c r="C21" s="74">
         <f>C20+1</f>
         <v/>
@@ -22521,7 +22527,9 @@
           <t>Gold</t>
         </is>
       </c>
-      <c r="B23" s="131" t="n"/>
+      <c r="B23" s="131" t="n">
+        <v>1881.7</v>
+      </c>
       <c r="C23" s="74">
         <f>C22+1</f>
         <v/>
@@ -22744,7 +22752,9 @@
           <t>Crude Oil</t>
         </is>
       </c>
-      <c r="B24" s="131" t="n"/>
+      <c r="B24" s="131" t="n">
+        <v>48.18</v>
+      </c>
       <c r="C24" s="74">
         <f>C23+1</f>
         <v/>
@@ -22997,7 +23007,9 @@
           <t>3-Month T-Bill</t>
         </is>
       </c>
-      <c r="B26" s="131" t="n"/>
+      <c r="B26" s="131" t="n">
+        <v>0.11</v>
+      </c>
       <c r="C26" s="74">
         <f>C25+1</f>
         <v/>
@@ -23220,7 +23232,9 @@
           <t>2-year Treasury</t>
         </is>
       </c>
-      <c r="B27" s="131" t="n"/>
+      <c r="B27" s="131" t="n">
+        <v>0.17</v>
+      </c>
       <c r="C27" s="74">
         <f>C26+1</f>
         <v/>
@@ -23443,7 +23457,9 @@
           <t>10-yr Treasury</t>
         </is>
       </c>
-      <c r="B28" s="131" t="n"/>
+      <c r="B28" s="131" t="n">
+        <v>1.46</v>
+      </c>
       <c r="C28" s="74">
         <f>C27+1</f>
         <v/>
@@ -23668,7 +23684,9 @@
           <t>30-year Treasury</t>
         </is>
       </c>
-      <c r="B29" s="131" t="n"/>
+      <c r="B29" s="131" t="n">
+        <v>1.67</v>
+      </c>
       <c r="C29" s="74">
         <f>C28+1</f>
         <v/>

</xml_diff>